<commit_message>
App for Spring started. good luck.
</commit_message>
<xml_diff>
--- a/spring_be_realistic.xlsx
+++ b/spring_be_realistic.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="96">
   <si>
     <t>Univ</t>
   </si>
@@ -745,6 +745,26 @@
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>추천서를 하드카피로 보내야된다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>waterloo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Toronto</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Western ontario</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Northeastern University Nov 15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -753,7 +773,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="m&quot;월&quot;\ d&quot;일&quot;"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -886,15 +906,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
@@ -931,7 +942,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -995,15 +1006,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1312,7 +1320,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1361,6 +1369,9 @@
       <c r="B2" s="18" t="s">
         <v>89</v>
       </c>
+      <c r="E2" s="2" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="3" spans="1:8" ht="100.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
@@ -1369,19 +1380,13 @@
       <c r="B3" s="17"/>
     </row>
     <row r="4" spans="1:8" ht="112.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="10"/>
+      <c r="A4" s="10" t="s">
+        <v>95</v>
+      </c>
       <c r="B4" s="17"/>
     </row>
-    <row r="5" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="9"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="9"/>
-      <c r="B9" s="17"/>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="24"/>
     </row>
     <row r="10" spans="1:8" s="12" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
@@ -1389,21 +1394,30 @@
     </row>
     <row r="11" spans="1:8" s="12" customFormat="1" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
-      <c r="B11" s="23"/>
-    </row>
-    <row r="12" spans="1:8" s="12" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="14"/>
-      <c r="B12" s="19"/>
-    </row>
-    <row r="13" spans="1:8" s="12" customFormat="1" ht="75.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="14"/>
-      <c r="B13" s="19"/>
-    </row>
-    <row r="14" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A14" s="22"/>
-    </row>
-    <row r="16" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A16" s="24"/>
+      <c r="B11" s="22"/>
+    </row>
+    <row r="12" spans="1:8" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B12" s="17"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="9"/>
+      <c r="B16" s="17"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="9"/>
@@ -1413,7 +1427,7 @@
       <c r="A18" s="11"/>
     </row>
     <row r="19" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A19" s="25"/>
+      <c r="A19" s="23"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="11"/>

</xml_diff>